<commit_message>
update: add pmd filtering; updated excel plots
</commit_message>
<xml_diff>
--- a/temp figs.xlsx
+++ b/temp figs.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="8_{4C8B5679-8E33-D44E-B831-3F2CAE5793B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{439510A7-263A-794A-8366-07FF1D6CB461}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18960" activeTab="1" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7546,8 +7546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D31A59-316A-8C46-8B17-B2E0BAD47F57}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="184" workbookViewId="0">
-      <selection activeCell="N71" sqref="N71"/>
+    <sheetView zoomScale="184" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8314,8 +8314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5697BF0-3995-194D-A4BB-9D78AC7A358A}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:S19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update: scrappy 230307 figs
</commit_message>
<xml_diff>
--- a/temp figs.xlsx
+++ b/temp figs.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="436" documentId="8_{4C8B5679-8E33-D44E-B831-3F2CAE5793B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF559B40-1A39-314A-9D03-757A0334BAB5}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="500" windowWidth="22300" windowHeight="18960" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
   </bookViews>
   <sheets>
     <sheet name="A mass+dev log1, most adults" sheetId="4" r:id="rId1"/>
@@ -23943,8 +23943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1009B4A-6CE7-0844-99E8-7A1384AD9D25}">
   <dimension ref="A1:AG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D92" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="115" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25792,7 +25792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D31A59-316A-8C46-8B17-B2E0BAD47F57}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="57" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="116" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update: tweaks to temp figs
</commit_message>
<xml_diff>
--- a/temp figs.xlsx
+++ b/temp figs.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="436" documentId="8_{4C8B5679-8E33-D44E-B831-3F2CAE5793B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF559B40-1A39-314A-9D03-757A0334BAB5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
+    <workbookView xWindow="1760" yWindow="500" windowWidth="31840" windowHeight="18960" xr2:uid="{84017D10-4509-084C-9811-4FC86B7B78D6}"/>
   </bookViews>
   <sheets>
     <sheet name="A mass+dev log1, most adults" sheetId="4" r:id="rId1"/>
@@ -23943,8 +23943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1009B4A-6CE7-0844-99E8-7A1384AD9D25}">
   <dimension ref="A1:AG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="115" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="115" workbookViewId="0">
+      <selection activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>